<commit_message>
further exploration into what makes a player HOF worthy
</commit_message>
<xml_diff>
--- a/projects/MLB_HOF_Predict/Data/myHOFCorr.xlsx
+++ b/projects/MLB_HOF_Predict/Data/myHOFCorr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="22">
   <si>
     <t>yearid</t>
   </si>
@@ -55,10 +55,28 @@
     <t>IBB</t>
   </si>
   <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>BattingAvg</t>
+  </si>
+  <si>
     <t>AllStarStarts</t>
   </si>
   <si>
     <t>AllStarGames</t>
+  </si>
+  <si>
+    <t>GoldGlove</t>
+  </si>
+  <si>
+    <t>TSNAllStar</t>
+  </si>
+  <si>
+    <t>MVP</t>
+  </si>
+  <si>
+    <t>SilverSlugger</t>
   </si>
   <si>
     <t>percentOfVotes</t>
@@ -419,13 +437,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:23">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,8 +492,26 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -483,843 +519,1557 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.7546552204707527</v>
+        <v>0.3149804012487367</v>
       </c>
       <c r="D2">
-        <v>0.7545900321943357</v>
+        <v>0.314038194718989</v>
       </c>
       <c r="E2">
-        <v>0.6893154174864552</v>
+        <v>0.2810503029531444</v>
       </c>
       <c r="F2">
-        <v>0.1171687528837906</v>
+        <v>0.1138292278711688</v>
       </c>
       <c r="G2">
-        <v>0.1652898611783296</v>
+        <v>-0.02891746198818941</v>
       </c>
       <c r="H2">
-        <v>-0.08213505526083262</v>
+        <v>0.07984966316441199</v>
       </c>
       <c r="I2">
-        <v>-0.06972871664664694</v>
+        <v>0.01843452655618737</v>
       </c>
       <c r="J2">
-        <v>0.2466265750712223</v>
+        <v>-0.006441695460564542</v>
       </c>
       <c r="K2">
-        <v>0.2706574373572115</v>
+        <v>0.175250459076274</v>
       </c>
       <c r="L2">
-        <v>-0.2876778461034595</v>
+        <v>-0.3337273210030334</v>
       </c>
       <c r="M2">
-        <v>-0.01966957084108643</v>
+        <v>-0.01921702532659272</v>
       </c>
       <c r="N2">
-        <v>0.2037063562384211</v>
+        <v>-0.1525517298258365</v>
       </c>
       <c r="O2">
-        <v>-0.197471385554462</v>
+        <v>-0.1495097334386069</v>
       </c>
       <c r="P2">
-        <v>-0.3957078428240083</v>
+        <v>0.3083098000054875</v>
       </c>
       <c r="Q2">
-        <v>0.06938150698324219</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
+        <v>-0.006129246048779525</v>
+      </c>
+      <c r="R2">
+        <v>-0.1364782902563462</v>
+      </c>
+      <c r="S2">
+        <v>-0.01142697623694329</v>
+      </c>
+      <c r="T2">
+        <v>0.1034280233213387</v>
+      </c>
+      <c r="U2">
+        <v>-0.2453395807318589</v>
+      </c>
+      <c r="V2">
+        <v>0.2133778137072049</v>
+      </c>
+      <c r="W2">
+        <v>0.0496037121616328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.7546552204707527</v>
+        <v>0.3149804012487367</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.9999839842196853</v>
+        <v>0.9999702435733371</v>
       </c>
       <c r="E3">
-        <v>0.8878732324755565</v>
+        <v>0.7606503385246479</v>
       </c>
       <c r="F3">
-        <v>0.1786997660495908</v>
+        <v>0.1172717394207783</v>
       </c>
       <c r="G3">
-        <v>0.2812623639870174</v>
+        <v>0.2121045605318079</v>
       </c>
       <c r="H3">
-        <v>-0.1535750192141587</v>
+        <v>-0.2793168746272268</v>
       </c>
       <c r="I3">
-        <v>-0.07913165263420004</v>
+        <v>-0.1511191648369708</v>
       </c>
       <c r="J3">
-        <v>0.2931516649156856</v>
+        <v>0.0819325916932875</v>
       </c>
       <c r="K3">
-        <v>0.286285345041202</v>
+        <v>0.2616190533821843</v>
       </c>
       <c r="L3">
-        <v>-0.09045417487017787</v>
+        <v>0.06722520191663098</v>
       </c>
       <c r="M3">
-        <v>-0.03125996433653104</v>
+        <v>-0.1026387176473602</v>
       </c>
       <c r="N3">
-        <v>0.1183801207302138</v>
+        <v>-0.4523863257731299</v>
       </c>
       <c r="O3">
-        <v>-0.07850075015343165</v>
+        <v>0.1563476146254171</v>
       </c>
       <c r="P3">
-        <v>-0.2193643651512952</v>
+        <v>0.03014031819544368</v>
       </c>
       <c r="Q3">
-        <v>0.02376613722190133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>0.1057162514274872</v>
+      </c>
+      <c r="R3">
+        <v>0.09848929908277083</v>
+      </c>
+      <c r="S3">
+        <v>-0.2988691215761641</v>
+      </c>
+      <c r="T3">
+        <v>0.09540061965465596</v>
+      </c>
+      <c r="U3">
+        <v>0.1316125008302108</v>
+      </c>
+      <c r="V3">
+        <v>0.2145733839081075</v>
+      </c>
+      <c r="W3">
+        <v>-0.09650142779952237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.7545900321943357</v>
+        <v>0.314038194718989</v>
       </c>
       <c r="C4">
-        <v>0.9999839842196853</v>
+        <v>0.9999702435733371</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.8875619023194983</v>
+        <v>0.7598995682149488</v>
       </c>
       <c r="F4">
-        <v>0.1792399271874446</v>
+        <v>0.1177936466430118</v>
       </c>
       <c r="G4">
-        <v>0.2818442230704681</v>
+        <v>0.2126976675454052</v>
       </c>
       <c r="H4">
-        <v>-0.152796479564366</v>
+        <v>-0.2785848166414926</v>
       </c>
       <c r="I4">
-        <v>-0.07820854640213649</v>
+        <v>-0.1499070868761867</v>
       </c>
       <c r="J4">
-        <v>0.2936076667721132</v>
+        <v>0.08258784821377123</v>
       </c>
       <c r="K4">
-        <v>0.2865051335269413</v>
+        <v>0.2618507171067115</v>
       </c>
       <c r="L4">
-        <v>-0.09032851700669275</v>
+        <v>0.06800543423225794</v>
       </c>
       <c r="M4">
-        <v>-0.03139285140523232</v>
+        <v>-0.1031738656520891</v>
       </c>
       <c r="N4">
-        <v>0.1188623908327618</v>
+        <v>-0.452805189118921</v>
       </c>
       <c r="O4">
-        <v>-0.07936219417996514</v>
+        <v>0.1568059867663545</v>
       </c>
       <c r="P4">
-        <v>-0.2199438252529583</v>
+        <v>0.03004177551278709</v>
       </c>
       <c r="Q4">
-        <v>0.02325861367776123</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>0.1043779259288262</v>
+      </c>
+      <c r="R4">
+        <v>0.09773941950847041</v>
+      </c>
+      <c r="S4">
+        <v>-0.2992610426321937</v>
+      </c>
+      <c r="T4">
+        <v>0.09242540704825832</v>
+      </c>
+      <c r="U4">
+        <v>0.1290931932376644</v>
+      </c>
+      <c r="V4">
+        <v>0.2121072891286565</v>
+      </c>
+      <c r="W4">
+        <v>-0.09750074432413595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.6893154174864552</v>
+        <v>0.2810503029531444</v>
       </c>
       <c r="C5">
-        <v>0.8878732324755565</v>
+        <v>0.7606503385246479</v>
       </c>
       <c r="D5">
-        <v>0.8875619023194983</v>
+        <v>0.7598995682149488</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>0.3722771040465717</v>
+        <v>0.3299475189349306</v>
       </c>
       <c r="G5">
-        <v>0.4390871290710468</v>
+        <v>0.3395528006297038</v>
       </c>
       <c r="H5">
-        <v>-0.04574591199485242</v>
+        <v>-0.1713338521752262</v>
       </c>
       <c r="I5">
-        <v>0.07377259600816687</v>
+        <v>-0.02438385285918619</v>
       </c>
       <c r="J5">
-        <v>0.3132990984501136</v>
+        <v>0.1220911597825965</v>
       </c>
       <c r="K5">
-        <v>0.4388748671918867</v>
+        <v>0.4049796202916724</v>
       </c>
       <c r="L5">
-        <v>-0.05710762689499579</v>
+        <v>-0.02528753633460103</v>
       </c>
       <c r="M5">
-        <v>0.1680557872614981</v>
+        <v>0.1978435737109921</v>
       </c>
       <c r="N5">
-        <v>0.3060795630380929</v>
+        <v>-0.1143798218474956</v>
       </c>
       <c r="O5">
-        <v>0.1624861527925358</v>
+        <v>0.2550915409077384</v>
       </c>
       <c r="P5">
-        <v>0.04670171787129977</v>
+        <v>0.2583920064014595</v>
       </c>
       <c r="Q5">
-        <v>0.475955375220797</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>0.3732742753505306</v>
+      </c>
+      <c r="R5">
+        <v>0.4279608338415831</v>
+      </c>
+      <c r="S5">
+        <v>-0.2061588681822478</v>
+      </c>
+      <c r="T5">
+        <v>0.2295275837840516</v>
+      </c>
+      <c r="U5">
+        <v>0.2229443983598271</v>
+      </c>
+      <c r="V5">
+        <v>0.2349099842058277</v>
+      </c>
+      <c r="W5">
+        <v>0.5698137200507941</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.1171687528837906</v>
+        <v>0.1138292278711688</v>
       </c>
       <c r="C6">
-        <v>0.1786997660495908</v>
+        <v>0.1172717394207783</v>
       </c>
       <c r="D6">
-        <v>0.1792399271874446</v>
+        <v>0.1177936466430118</v>
       </c>
       <c r="E6">
-        <v>0.3722771040465717</v>
+        <v>0.3299475189349306</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.8047106148000652</v>
+        <v>0.693926739211661</v>
       </c>
       <c r="H6">
-        <v>0.370960543994681</v>
+        <v>0.04767069620798248</v>
       </c>
       <c r="I6">
-        <v>0.5105832765132142</v>
+        <v>0.1495264841043777</v>
       </c>
       <c r="J6">
-        <v>0.4589527775448945</v>
+        <v>0.5772527062518975</v>
       </c>
       <c r="K6">
-        <v>0.7092353082325273</v>
+        <v>0.665669021620928</v>
       </c>
       <c r="L6">
-        <v>0.4139980071566069</v>
+        <v>0.2600308158090338</v>
       </c>
       <c r="M6">
-        <v>0.6998337639621656</v>
+        <v>0.6956357225612111</v>
       </c>
       <c r="N6">
-        <v>0.3575645196227772</v>
+        <v>-0.0487008002203436</v>
       </c>
       <c r="O6">
-        <v>0.2799129590183152</v>
+        <v>0.7453222916384522</v>
       </c>
       <c r="P6">
-        <v>0.3570771091835725</v>
+        <v>0.2498130726512735</v>
       </c>
       <c r="Q6">
-        <v>0.5131285934563975</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>-0.1037281357809414</v>
+      </c>
+      <c r="R6">
+        <v>-0.04251344973848595</v>
+      </c>
+      <c r="S6">
+        <v>-0.3061221156004067</v>
+      </c>
+      <c r="T6">
+        <v>-0.3547145787261782</v>
+      </c>
+      <c r="U6">
+        <v>0.02301028553399298</v>
+      </c>
+      <c r="V6">
+        <v>-0.3000750156823546</v>
+      </c>
+      <c r="W6">
+        <v>0.354488668441156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.1652898611783296</v>
+        <v>-0.02891746198818941</v>
       </c>
       <c r="C7">
-        <v>0.2812623639870174</v>
+        <v>0.2121045605318079</v>
       </c>
       <c r="D7">
-        <v>0.2818442230704681</v>
+        <v>0.2126976675454052</v>
       </c>
       <c r="E7">
-        <v>0.4390871290710468</v>
+        <v>0.3395528006297038</v>
       </c>
       <c r="F7">
-        <v>0.8047106148000652</v>
+        <v>0.693926739211661</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7">
-        <v>0.1095359035850467</v>
+        <v>-0.2239580081794407</v>
       </c>
       <c r="I7">
-        <v>0.4479541854539091</v>
+        <v>0.131078824552251</v>
       </c>
       <c r="J7">
-        <v>0.3059523060243322</v>
+        <v>0.2836966635693545</v>
       </c>
       <c r="K7">
-        <v>0.8860331552148636</v>
+        <v>0.8560183015010304</v>
       </c>
       <c r="L7">
-        <v>0.5648627009748086</v>
+        <v>0.4938688271265019</v>
       </c>
       <c r="M7">
-        <v>0.2934789692031198</v>
+        <v>0.1785768655267361</v>
       </c>
       <c r="N7">
-        <v>0.4031680357506008</v>
+        <v>0.04222249303140569</v>
       </c>
       <c r="O7">
-        <v>0.3558893513644792</v>
+        <v>0.8980998924255382</v>
       </c>
       <c r="P7">
-        <v>0.4159991007577096</v>
+        <v>0.1711298071628818</v>
       </c>
       <c r="Q7">
-        <v>0.4646681024900934</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>0.09804764096089644</v>
+      </c>
+      <c r="R7">
+        <v>0.2017234705422877</v>
+      </c>
+      <c r="S7">
+        <v>-0.2531665324210869</v>
+      </c>
+      <c r="T7">
+        <v>-0.2917564845157683</v>
+      </c>
+      <c r="U7">
+        <v>-0.1735647408886047</v>
+      </c>
+      <c r="V7">
+        <v>-0.005841529776130068</v>
+      </c>
+      <c r="W7">
+        <v>0.2379017629808265</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.08213505526083262</v>
+        <v>0.07984966316441199</v>
       </c>
       <c r="C8">
-        <v>-0.1535750192141587</v>
+        <v>-0.2793168746272268</v>
       </c>
       <c r="D8">
-        <v>-0.152796479564366</v>
+        <v>-0.2785848166414926</v>
       </c>
       <c r="E8">
-        <v>-0.04574591199485242</v>
+        <v>-0.1713338521752262</v>
       </c>
       <c r="F8">
-        <v>0.370960543994681</v>
+        <v>0.04767069620798248</v>
       </c>
       <c r="G8">
-        <v>0.1095359035850467</v>
+        <v>-0.2239580081794407</v>
       </c>
       <c r="H8">
         <v>1</v>
       </c>
       <c r="I8">
-        <v>0.8812440411434715</v>
+        <v>0.8871011895921911</v>
       </c>
       <c r="J8">
-        <v>-0.3831537138804358</v>
+        <v>-0.4944851888555465</v>
       </c>
       <c r="K8">
-        <v>0.07434894998266794</v>
+        <v>-0.04949041626859068</v>
       </c>
       <c r="L8">
-        <v>-0.2272446969586334</v>
+        <v>-0.5683215081754912</v>
       </c>
       <c r="M8">
-        <v>0.4549621539149601</v>
+        <v>0.2928436620748339</v>
       </c>
       <c r="N8">
-        <v>0.6023759383533109</v>
+        <v>0.5385425648404144</v>
       </c>
       <c r="O8">
-        <v>0.1204255925941881</v>
+        <v>-0.04623085841278701</v>
       </c>
       <c r="P8">
-        <v>0.2289121048603613</v>
+        <v>-0.1242483147850396</v>
       </c>
       <c r="Q8">
-        <v>0.2430025505314354</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>-0.218779854244646</v>
+      </c>
+      <c r="R8">
+        <v>-0.1955065296947023</v>
+      </c>
+      <c r="S8">
+        <v>0.02883378361535878</v>
+      </c>
+      <c r="T8">
+        <v>-0.06936434345973858</v>
+      </c>
+      <c r="U8">
+        <v>0.112874547262103</v>
+      </c>
+      <c r="V8">
+        <v>-0.02229874244715696</v>
+      </c>
+      <c r="W8">
+        <v>0.1168017967115797</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>-0.06972871664664694</v>
+        <v>0.01843452655618737</v>
       </c>
       <c r="C9">
-        <v>-0.07913165263420004</v>
+        <v>-0.1511191648369708</v>
       </c>
       <c r="D9">
-        <v>-0.07820854640213649</v>
+        <v>-0.1499070868761867</v>
       </c>
       <c r="E9">
-        <v>0.07377259600816687</v>
+        <v>-0.02438385285918619</v>
       </c>
       <c r="F9">
-        <v>0.5105832765132142</v>
+        <v>0.1495264841043777</v>
       </c>
       <c r="G9">
-        <v>0.4479541854539091</v>
+        <v>0.131078824552251</v>
       </c>
       <c r="H9">
-        <v>0.8812440411434715</v>
+        <v>0.8871011895921911</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="J9">
-        <v>-0.3887652954360826</v>
+        <v>-0.551445594525184</v>
       </c>
       <c r="K9">
-        <v>0.4356385581831733</v>
+        <v>0.264791190024384</v>
       </c>
       <c r="L9">
-        <v>0.01019461912677449</v>
+        <v>-0.3688647206978435</v>
       </c>
       <c r="M9">
-        <v>0.4223150749661975</v>
+        <v>0.2623560250468696</v>
       </c>
       <c r="N9">
-        <v>0.654702956063843</v>
+        <v>0.5969216815837375</v>
       </c>
       <c r="O9">
-        <v>0.2214125803897782</v>
+        <v>0.2528996055368141</v>
       </c>
       <c r="P9">
-        <v>0.3561962302539116</v>
+        <v>-0.08430449844630898</v>
       </c>
       <c r="Q9">
-        <v>0.3743539392119143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>-0.1715817387964316</v>
+      </c>
+      <c r="R9">
+        <v>-0.07711932963465372</v>
+      </c>
+      <c r="S9">
+        <v>-0.05816580722627542</v>
+      </c>
+      <c r="T9">
+        <v>-0.1861055575269345</v>
+      </c>
+      <c r="U9">
+        <v>0.08787433499787142</v>
+      </c>
+      <c r="V9">
+        <v>-0.05720319775745537</v>
+      </c>
+      <c r="W9">
+        <v>0.1743607284081984</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.2466265750712223</v>
+        <v>-0.006441695460564542</v>
       </c>
       <c r="C10">
-        <v>0.2931516649156856</v>
+        <v>0.0819325916932875</v>
       </c>
       <c r="D10">
-        <v>0.2936076667721132</v>
+        <v>0.08258784821377123</v>
       </c>
       <c r="E10">
-        <v>0.3132990984501136</v>
+        <v>0.1220911597825965</v>
       </c>
       <c r="F10">
-        <v>0.4589527775448945</v>
+        <v>0.5772527062518975</v>
       </c>
       <c r="G10">
-        <v>0.3059523060243322</v>
+        <v>0.2836966635693545</v>
       </c>
       <c r="H10">
-        <v>-0.3831537138804358</v>
+        <v>-0.4944851888555465</v>
       </c>
       <c r="I10">
-        <v>-0.3887652954360826</v>
+        <v>-0.551445594525184</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0.17286534516123</v>
+        <v>0.08604619101023843</v>
       </c>
       <c r="L10">
-        <v>0.3809266907690799</v>
+        <v>0.5020612381814391</v>
       </c>
       <c r="M10">
-        <v>0.2169924127479998</v>
+        <v>0.2888020728771696</v>
       </c>
       <c r="N10">
-        <v>-0.1680218762640607</v>
+        <v>-0.4224754960967472</v>
       </c>
       <c r="O10">
-        <v>-0.04369475215059521</v>
+        <v>0.3188849419884965</v>
       </c>
       <c r="P10">
-        <v>-0.09137253824343401</v>
+        <v>0.05117789487909899</v>
       </c>
       <c r="Q10">
-        <v>0.1097533154629201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>-0.05569328198363838</v>
+      </c>
+      <c r="R10">
+        <v>-0.04487510836204685</v>
+      </c>
+      <c r="S10">
+        <v>-0.05503523057189239</v>
+      </c>
+      <c r="T10">
+        <v>-0.2849758248641258</v>
+      </c>
+      <c r="U10">
+        <v>-0.09516159816636967</v>
+      </c>
+      <c r="V10">
+        <v>-0.3309658359918066</v>
+      </c>
+      <c r="W10">
+        <v>0.06379619565887278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.2706574373572115</v>
+        <v>0.175250459076274</v>
       </c>
       <c r="C11">
-        <v>0.286285345041202</v>
+        <v>0.2616190533821843</v>
       </c>
       <c r="D11">
-        <v>0.2865051335269413</v>
+        <v>0.2618507171067115</v>
       </c>
       <c r="E11">
-        <v>0.4388748671918867</v>
+        <v>0.4049796202916724</v>
       </c>
       <c r="F11">
-        <v>0.7092353082325273</v>
+        <v>0.665669021620928</v>
       </c>
       <c r="G11">
-        <v>0.8860331552148636</v>
+        <v>0.8560183015010304</v>
       </c>
       <c r="H11">
-        <v>0.07434894998266794</v>
+        <v>-0.04949041626859068</v>
       </c>
       <c r="I11">
-        <v>0.4356385581831733</v>
+        <v>0.264791190024384</v>
       </c>
       <c r="J11">
-        <v>0.17286534516123</v>
+        <v>0.08604619101023843</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11">
-        <v>0.4452231702697098</v>
+        <v>0.2661155159066899</v>
       </c>
       <c r="M11">
-        <v>0.2659657758008068</v>
+        <v>0.222126668492748</v>
       </c>
       <c r="N11">
-        <v>0.3161207300460843</v>
+        <v>0.06533379255210943</v>
       </c>
       <c r="O11">
-        <v>0.229740060874199</v>
+        <v>0.7816510685122006</v>
       </c>
       <c r="P11">
-        <v>0.2454059647185816</v>
+        <v>0.1842752304292082</v>
       </c>
       <c r="Q11">
-        <v>0.44666362656677</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>0.04260146385650507</v>
+      </c>
+      <c r="R11">
+        <v>0.1126632309762068</v>
+      </c>
+      <c r="S11">
+        <v>-0.2946195408401093</v>
+      </c>
+      <c r="T11">
+        <v>-0.2654331624711819</v>
+      </c>
+      <c r="U11">
+        <v>-0.09144712226617431</v>
+      </c>
+      <c r="V11">
+        <v>0.02970574894098682</v>
+      </c>
+      <c r="W11">
+        <v>0.2829360861445329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>-0.2876778461034595</v>
+        <v>-0.3337273210030334</v>
       </c>
       <c r="C12">
-        <v>-0.09045417487017787</v>
+        <v>0.06722520191663098</v>
       </c>
       <c r="D12">
-        <v>-0.09032851700669275</v>
+        <v>0.06800543423225794</v>
       </c>
       <c r="E12">
-        <v>-0.05710762689499579</v>
+        <v>-0.02528753633460103</v>
       </c>
       <c r="F12">
-        <v>0.4139980071566069</v>
+        <v>0.2600308158090338</v>
       </c>
       <c r="G12">
-        <v>0.5648627009748086</v>
+        <v>0.4938688271265019</v>
       </c>
       <c r="H12">
-        <v>-0.2272446969586334</v>
+        <v>-0.5683215081754912</v>
       </c>
       <c r="I12">
-        <v>0.01019461912677449</v>
+        <v>-0.3688647206978435</v>
       </c>
       <c r="J12">
-        <v>0.3809266907690799</v>
+        <v>0.5020612381814391</v>
       </c>
       <c r="K12">
-        <v>0.4452231702697098</v>
+        <v>0.2661155159066899</v>
       </c>
       <c r="L12">
         <v>1</v>
       </c>
       <c r="M12">
-        <v>-0.0285633098112071</v>
+        <v>-0.1713586347178806</v>
       </c>
       <c r="N12">
-        <v>-0.02732838142837331</v>
+        <v>-0.1794966406851852</v>
       </c>
       <c r="O12">
-        <v>0.1965451503807369</v>
+        <v>0.4103881440229643</v>
       </c>
       <c r="P12">
-        <v>0.2585046190742597</v>
+        <v>-0.04488421671721288</v>
       </c>
       <c r="Q12">
-        <v>0.07173027060941578</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>-0.08673560676058246</v>
+      </c>
+      <c r="R12">
+        <v>-0.06272085777250985</v>
+      </c>
+      <c r="S12">
+        <v>-0.1387898921112558</v>
+      </c>
+      <c r="T12">
+        <v>-0.2633572592246277</v>
+      </c>
+      <c r="U12">
+        <v>-0.08083443892603095</v>
+      </c>
+      <c r="V12">
+        <v>-0.2519984679359923</v>
+      </c>
+      <c r="W12">
+        <v>-0.1440647329950141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>-0.01966957084108643</v>
+        <v>-0.01921702532659272</v>
       </c>
       <c r="C13">
-        <v>-0.03125996433653104</v>
+        <v>-0.1026387176473602</v>
       </c>
       <c r="D13">
-        <v>-0.03139285140523232</v>
+        <v>-0.1031738656520891</v>
       </c>
       <c r="E13">
-        <v>0.1680557872614981</v>
+        <v>0.1978435737109921</v>
       </c>
       <c r="F13">
-        <v>0.6998337639621656</v>
+        <v>0.6956357225612111</v>
       </c>
       <c r="G13">
-        <v>0.2934789692031198</v>
+        <v>0.1785768655267361</v>
       </c>
       <c r="H13">
-        <v>0.4549621539149601</v>
+        <v>0.2928436620748339</v>
       </c>
       <c r="I13">
-        <v>0.4223150749661975</v>
+        <v>0.2623560250468696</v>
       </c>
       <c r="J13">
-        <v>0.2169924127479998</v>
+        <v>0.2888020728771696</v>
       </c>
       <c r="K13">
-        <v>0.2659657758008068</v>
+        <v>0.222126668492748</v>
       </c>
       <c r="L13">
-        <v>-0.0285633098112071</v>
+        <v>-0.1713586347178806</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13">
-        <v>0.308699122038181</v>
+        <v>0.1899119558770747</v>
       </c>
       <c r="O13">
-        <v>0.08214083911633047</v>
+        <v>0.3020851105154888</v>
       </c>
       <c r="P13">
-        <v>0.2051654059502223</v>
+        <v>0.3839510374096216</v>
       </c>
       <c r="Q13">
-        <v>0.4456198063854278</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17">
+        <v>-0.1501339836422558</v>
+      </c>
+      <c r="R13">
+        <v>-0.05096122707349294</v>
+      </c>
+      <c r="S13">
+        <v>-0.2609122585451593</v>
+      </c>
+      <c r="T13">
+        <v>-0.2669828757252486</v>
+      </c>
+      <c r="U13">
+        <v>0.2197361045156079</v>
+      </c>
+      <c r="V13">
+        <v>-0.4312727352008251</v>
+      </c>
+      <c r="W13">
+        <v>0.4403667758553718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0.2037063562384211</v>
+        <v>-0.1525517298258365</v>
       </c>
       <c r="C14">
-        <v>0.1183801207302138</v>
+        <v>-0.4523863257731299</v>
       </c>
       <c r="D14">
-        <v>0.1188623908327618</v>
+        <v>-0.452805189118921</v>
       </c>
       <c r="E14">
-        <v>0.3060795630380929</v>
+        <v>-0.1143798218474956</v>
       </c>
       <c r="F14">
-        <v>0.3575645196227772</v>
+        <v>-0.0487008002203436</v>
       </c>
       <c r="G14">
-        <v>0.4031680357506008</v>
+        <v>0.04222249303140569</v>
       </c>
       <c r="H14">
-        <v>0.6023759383533109</v>
+        <v>0.5385425648404144</v>
       </c>
       <c r="I14">
-        <v>0.654702956063843</v>
+        <v>0.5969216815837375</v>
       </c>
       <c r="J14">
-        <v>-0.1680218762640607</v>
+        <v>-0.4224754960967472</v>
       </c>
       <c r="K14">
-        <v>0.3161207300460843</v>
+        <v>0.06533379255210943</v>
       </c>
       <c r="L14">
-        <v>-0.02732838142837331</v>
+        <v>-0.1794966406851852</v>
       </c>
       <c r="M14">
-        <v>0.308699122038181</v>
+        <v>0.1899119558770747</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
       <c r="O14">
-        <v>0.08279629615732813</v>
+        <v>-0.02750332510053873</v>
       </c>
       <c r="P14">
-        <v>0.1421216482194625</v>
+        <v>0.2677709180420111</v>
       </c>
       <c r="Q14">
-        <v>0.4714869252510766</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17">
+        <v>-0.1303460178969339</v>
+      </c>
+      <c r="R14">
+        <v>-0.05364407432482431</v>
+      </c>
+      <c r="S14">
+        <v>-0.06732810850887075</v>
+      </c>
+      <c r="T14">
+        <v>-0.1082508236766214</v>
+      </c>
+      <c r="U14">
+        <v>-0.08229598838334369</v>
+      </c>
+      <c r="V14">
+        <v>0.1005397832430474</v>
+      </c>
+      <c r="W14">
+        <v>0.3965815181597921</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
-        <v>-0.197471385554462</v>
+        <v>-0.1495097334386069</v>
       </c>
       <c r="C15">
-        <v>-0.07850075015343165</v>
+        <v>0.1563476146254171</v>
       </c>
       <c r="D15">
-        <v>-0.07936219417996514</v>
+        <v>0.1568059867663545</v>
       </c>
       <c r="E15">
-        <v>0.1624861527925358</v>
+        <v>0.2550915409077384</v>
       </c>
       <c r="F15">
-        <v>0.2799129590183152</v>
+        <v>0.7453222916384522</v>
       </c>
       <c r="G15">
-        <v>0.3558893513644792</v>
+        <v>0.8980998924255382</v>
       </c>
       <c r="H15">
-        <v>0.1204255925941881</v>
+        <v>-0.04623085841278701</v>
       </c>
       <c r="I15">
-        <v>0.2214125803897782</v>
+        <v>0.2528996055368141</v>
       </c>
       <c r="J15">
-        <v>-0.04369475215059521</v>
+        <v>0.3188849419884965</v>
       </c>
       <c r="K15">
-        <v>0.229740060874199</v>
+        <v>0.7816510685122006</v>
       </c>
       <c r="L15">
-        <v>0.1965451503807369</v>
+        <v>0.4103881440229643</v>
       </c>
       <c r="M15">
-        <v>0.08214083911633047</v>
+        <v>0.3020851105154888</v>
       </c>
       <c r="N15">
-        <v>0.08279629615732813</v>
+        <v>-0.02750332510053873</v>
       </c>
       <c r="O15">
         <v>1</v>
       </c>
       <c r="P15">
-        <v>0.8904812589271225</v>
+        <v>-0.1725239601677718</v>
       </c>
       <c r="Q15">
-        <v>0.5295668879163438</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17">
+        <v>0.05942524011069036</v>
+      </c>
+      <c r="R15">
+        <v>0.1861216401677274</v>
+      </c>
+      <c r="S15">
+        <v>-0.1848720450080256</v>
+      </c>
+      <c r="T15">
+        <v>-0.3763477161453859</v>
+      </c>
+      <c r="U15">
+        <v>-0.02172325633441028</v>
+      </c>
+      <c r="V15">
+        <v>-0.1897675039194066</v>
+      </c>
+      <c r="W15">
+        <v>0.1847688882509557</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
-        <v>-0.3957078428240083</v>
+        <v>0.3083098000054875</v>
       </c>
       <c r="C16">
-        <v>-0.2193643651512952</v>
+        <v>0.03014031819544368</v>
       </c>
       <c r="D16">
-        <v>-0.2199438252529583</v>
+        <v>0.03004177551278709</v>
       </c>
       <c r="E16">
-        <v>0.04670171787129977</v>
+        <v>0.2583920064014595</v>
       </c>
       <c r="F16">
-        <v>0.3570771091835725</v>
+        <v>0.2498130726512735</v>
       </c>
       <c r="G16">
-        <v>0.4159991007577096</v>
+        <v>0.1711298071628818</v>
       </c>
       <c r="H16">
-        <v>0.2289121048603613</v>
+        <v>-0.1242483147850396</v>
       </c>
       <c r="I16">
-        <v>0.3561962302539116</v>
+        <v>-0.08430449844630898</v>
       </c>
       <c r="J16">
-        <v>-0.09137253824343401</v>
+        <v>0.05117789487909899</v>
       </c>
       <c r="K16">
-        <v>0.2454059647185816</v>
+        <v>0.1842752304292082</v>
       </c>
       <c r="L16">
-        <v>0.2585046190742597</v>
+        <v>-0.04488421671721288</v>
       </c>
       <c r="M16">
-        <v>0.2051654059502223</v>
+        <v>0.3839510374096216</v>
       </c>
       <c r="N16">
-        <v>0.1421216482194625</v>
+        <v>0.2677709180420111</v>
       </c>
       <c r="O16">
-        <v>0.8904812589271225</v>
+        <v>-0.1725239601677718</v>
       </c>
       <c r="P16">
         <v>1</v>
       </c>
       <c r="Q16">
-        <v>0.5543786094523636</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17">
+        <v>-0.04927268895336187</v>
+      </c>
+      <c r="R16">
+        <v>-0.07395841647987875</v>
+      </c>
+      <c r="S16">
+        <v>-0.3185535534862392</v>
+      </c>
+      <c r="T16">
+        <v>0.03954110143115101</v>
+      </c>
+      <c r="U16">
+        <v>-0.1047592513005594</v>
+      </c>
+      <c r="V16">
+        <v>0.0952222487997965</v>
+      </c>
+      <c r="W16">
+        <v>0.3536459688180477</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0.06938150698324219</v>
+        <v>-0.006129246048779525</v>
       </c>
       <c r="C17">
-        <v>0.02376613722190133</v>
+        <v>0.1057162514274872</v>
       </c>
       <c r="D17">
-        <v>0.02325861367776123</v>
+        <v>0.1043779259288262</v>
       </c>
       <c r="E17">
-        <v>0.475955375220797</v>
+        <v>0.3732742753505306</v>
       </c>
       <c r="F17">
-        <v>0.5131285934563975</v>
+        <v>-0.1037281357809414</v>
       </c>
       <c r="G17">
-        <v>0.4646681024900934</v>
+        <v>0.09804764096089644</v>
       </c>
       <c r="H17">
-        <v>0.2430025505314354</v>
+        <v>-0.218779854244646</v>
       </c>
       <c r="I17">
-        <v>0.3743539392119143</v>
+        <v>-0.1715817387964316</v>
       </c>
       <c r="J17">
-        <v>0.1097533154629201</v>
+        <v>-0.05569328198363838</v>
       </c>
       <c r="K17">
-        <v>0.44666362656677</v>
+        <v>0.04260146385650507</v>
       </c>
       <c r="L17">
-        <v>0.07173027060941578</v>
+        <v>-0.08673560676058246</v>
       </c>
       <c r="M17">
-        <v>0.4456198063854278</v>
+        <v>-0.1501339836422558</v>
       </c>
       <c r="N17">
-        <v>0.4714869252510766</v>
+        <v>-0.1303460178969339</v>
       </c>
       <c r="O17">
-        <v>0.5295668879163438</v>
+        <v>0.05942524011069036</v>
       </c>
       <c r="P17">
-        <v>0.5543786094523636</v>
+        <v>-0.04927268895336187</v>
       </c>
       <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>0.8828948126040759</v>
+      </c>
+      <c r="S17">
+        <v>0.3595508975908289</v>
+      </c>
+      <c r="T17">
+        <v>0.6536566525076064</v>
+      </c>
+      <c r="U17">
+        <v>0.02292436144110454</v>
+      </c>
+      <c r="V17">
+        <v>0.4740515041533957</v>
+      </c>
+      <c r="W17">
+        <v>0.433802636780796</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>-0.1364782902563462</v>
+      </c>
+      <c r="C18">
+        <v>0.09848929908277083</v>
+      </c>
+      <c r="D18">
+        <v>0.09773941950847041</v>
+      </c>
+      <c r="E18">
+        <v>0.4279608338415831</v>
+      </c>
+      <c r="F18">
+        <v>-0.04251344973848595</v>
+      </c>
+      <c r="G18">
+        <v>0.2017234705422877</v>
+      </c>
+      <c r="H18">
+        <v>-0.1955065296947023</v>
+      </c>
+      <c r="I18">
+        <v>-0.07711932963465372</v>
+      </c>
+      <c r="J18">
+        <v>-0.04487510836204685</v>
+      </c>
+      <c r="K18">
+        <v>0.1126632309762068</v>
+      </c>
+      <c r="L18">
+        <v>-0.06272085777250985</v>
+      </c>
+      <c r="M18">
+        <v>-0.05096122707349294</v>
+      </c>
+      <c r="N18">
+        <v>-0.05364407432482431</v>
+      </c>
+      <c r="O18">
+        <v>0.1861216401677274</v>
+      </c>
+      <c r="P18">
+        <v>-0.07395841647987875</v>
+      </c>
+      <c r="Q18">
+        <v>0.8828948126040759</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>0.3625644302121404</v>
+      </c>
+      <c r="T18">
+        <v>0.568364664691217</v>
+      </c>
+      <c r="U18">
+        <v>0.004257373359800774</v>
+      </c>
+      <c r="V18">
+        <v>0.4322417648926214</v>
+      </c>
+      <c r="W18">
+        <v>0.5310681561326083</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
+      <c r="A19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>-0.01142697623694329</v>
+      </c>
+      <c r="C19">
+        <v>-0.2988691215761641</v>
+      </c>
+      <c r="D19">
+        <v>-0.2992610426321937</v>
+      </c>
+      <c r="E19">
+        <v>-0.2061588681822478</v>
+      </c>
+      <c r="F19">
+        <v>-0.3061221156004067</v>
+      </c>
+      <c r="G19">
+        <v>-0.2531665324210869</v>
+      </c>
+      <c r="H19">
+        <v>0.02883378361535878</v>
+      </c>
+      <c r="I19">
+        <v>-0.05816580722627542</v>
+      </c>
+      <c r="J19">
+        <v>-0.05503523057189239</v>
+      </c>
+      <c r="K19">
+        <v>-0.2946195408401093</v>
+      </c>
+      <c r="L19">
+        <v>-0.1387898921112558</v>
+      </c>
+      <c r="M19">
+        <v>-0.2609122585451593</v>
+      </c>
+      <c r="N19">
+        <v>-0.06732810850887075</v>
+      </c>
+      <c r="O19">
+        <v>-0.1848720450080256</v>
+      </c>
+      <c r="P19">
+        <v>-0.3185535534862392</v>
+      </c>
+      <c r="Q19">
+        <v>0.3595508975908289</v>
+      </c>
+      <c r="R19">
+        <v>0.3625644302121404</v>
+      </c>
+      <c r="S19">
+        <v>1</v>
+      </c>
+      <c r="T19">
+        <v>0.283967415958102</v>
+      </c>
+      <c r="U19">
+        <v>0.09172815366298744</v>
+      </c>
+      <c r="V19">
+        <v>0.1046761429475829</v>
+      </c>
+      <c r="W19">
+        <v>0.02554550798784269</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>0.1034280233213387</v>
+      </c>
+      <c r="C20">
+        <v>0.09540061965465596</v>
+      </c>
+      <c r="D20">
+        <v>0.09242540704825832</v>
+      </c>
+      <c r="E20">
+        <v>0.2295275837840516</v>
+      </c>
+      <c r="F20">
+        <v>-0.3547145787261782</v>
+      </c>
+      <c r="G20">
+        <v>-0.2917564845157683</v>
+      </c>
+      <c r="H20">
+        <v>-0.06936434345973858</v>
+      </c>
+      <c r="I20">
+        <v>-0.1861055575269345</v>
+      </c>
+      <c r="J20">
+        <v>-0.2849758248641258</v>
+      </c>
+      <c r="K20">
+        <v>-0.2654331624711819</v>
+      </c>
+      <c r="L20">
+        <v>-0.2633572592246277</v>
+      </c>
+      <c r="M20">
+        <v>-0.2669828757252486</v>
+      </c>
+      <c r="N20">
+        <v>-0.1082508236766214</v>
+      </c>
+      <c r="O20">
+        <v>-0.3763477161453859</v>
+      </c>
+      <c r="P20">
+        <v>0.03954110143115101</v>
+      </c>
+      <c r="Q20">
+        <v>0.6536566525076064</v>
+      </c>
+      <c r="R20">
+        <v>0.568364664691217</v>
+      </c>
+      <c r="S20">
+        <v>0.283967415958102</v>
+      </c>
+      <c r="T20">
+        <v>1</v>
+      </c>
+      <c r="U20">
+        <v>0.3179881251307417</v>
+      </c>
+      <c r="V20">
+        <v>0.7517251372944621</v>
+      </c>
+      <c r="W20">
+        <v>0.2376083114873622</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>-0.2453395807318589</v>
+      </c>
+      <c r="C21">
+        <v>0.1316125008302108</v>
+      </c>
+      <c r="D21">
+        <v>0.1290931932376644</v>
+      </c>
+      <c r="E21">
+        <v>0.2229443983598271</v>
+      </c>
+      <c r="F21">
+        <v>0.02301028553399298</v>
+      </c>
+      <c r="G21">
+        <v>-0.1735647408886047</v>
+      </c>
+      <c r="H21">
+        <v>0.112874547262103</v>
+      </c>
+      <c r="I21">
+        <v>0.08787433499787142</v>
+      </c>
+      <c r="J21">
+        <v>-0.09516159816636967</v>
+      </c>
+      <c r="K21">
+        <v>-0.09144712226617431</v>
+      </c>
+      <c r="L21">
+        <v>-0.08083443892603095</v>
+      </c>
+      <c r="M21">
+        <v>0.2197361045156079</v>
+      </c>
+      <c r="N21">
+        <v>-0.08229598838334369</v>
+      </c>
+      <c r="O21">
+        <v>-0.02172325633441028</v>
+      </c>
+      <c r="P21">
+        <v>-0.1047592513005594</v>
+      </c>
+      <c r="Q21">
+        <v>0.02292436144110454</v>
+      </c>
+      <c r="R21">
+        <v>0.004257373359800774</v>
+      </c>
+      <c r="S21">
+        <v>0.09172815366298744</v>
+      </c>
+      <c r="T21">
+        <v>0.3179881251307417</v>
+      </c>
+      <c r="U21">
+        <v>1</v>
+      </c>
+      <c r="V21">
+        <v>0.004714045207910344</v>
+      </c>
+      <c r="W21">
+        <v>0.1507388802649037</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>0.2133778137072049</v>
+      </c>
+      <c r="C22">
+        <v>0.2145733839081075</v>
+      </c>
+      <c r="D22">
+        <v>0.2121072891286565</v>
+      </c>
+      <c r="E22">
+        <v>0.2349099842058277</v>
+      </c>
+      <c r="F22">
+        <v>-0.3000750156823546</v>
+      </c>
+      <c r="G22">
+        <v>-0.005841529776130068</v>
+      </c>
+      <c r="H22">
+        <v>-0.02229874244715696</v>
+      </c>
+      <c r="I22">
+        <v>-0.05720319775745537</v>
+      </c>
+      <c r="J22">
+        <v>-0.3309658359918066</v>
+      </c>
+      <c r="K22">
+        <v>0.02970574894098682</v>
+      </c>
+      <c r="L22">
+        <v>-0.2519984679359923</v>
+      </c>
+      <c r="M22">
+        <v>-0.4312727352008251</v>
+      </c>
+      <c r="N22">
+        <v>0.1005397832430474</v>
+      </c>
+      <c r="O22">
+        <v>-0.1897675039194066</v>
+      </c>
+      <c r="P22">
+        <v>0.0952222487997965</v>
+      </c>
+      <c r="Q22">
+        <v>0.4740515041533957</v>
+      </c>
+      <c r="R22">
+        <v>0.4322417648926214</v>
+      </c>
+      <c r="S22">
+        <v>0.1046761429475829</v>
+      </c>
+      <c r="T22">
+        <v>0.7517251372944621</v>
+      </c>
+      <c r="U22">
+        <v>0.004714045207910344</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>0.06359178652054678</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>0.0496037121616328</v>
+      </c>
+      <c r="C23">
+        <v>-0.09650142779952237</v>
+      </c>
+      <c r="D23">
+        <v>-0.09750074432413595</v>
+      </c>
+      <c r="E23">
+        <v>0.5698137200507941</v>
+      </c>
+      <c r="F23">
+        <v>0.354488668441156</v>
+      </c>
+      <c r="G23">
+        <v>0.2379017629808265</v>
+      </c>
+      <c r="H23">
+        <v>0.1168017967115797</v>
+      </c>
+      <c r="I23">
+        <v>0.1743607284081984</v>
+      </c>
+      <c r="J23">
+        <v>0.06379619565887278</v>
+      </c>
+      <c r="K23">
+        <v>0.2829360861445329</v>
+      </c>
+      <c r="L23">
+        <v>-0.1440647329950141</v>
+      </c>
+      <c r="M23">
+        <v>0.4403667758553718</v>
+      </c>
+      <c r="N23">
+        <v>0.3965815181597921</v>
+      </c>
+      <c r="O23">
+        <v>0.1847688882509557</v>
+      </c>
+      <c r="P23">
+        <v>0.3536459688180477</v>
+      </c>
+      <c r="Q23">
+        <v>0.433802636780796</v>
+      </c>
+      <c r="R23">
+        <v>0.5310681561326083</v>
+      </c>
+      <c r="S23">
+        <v>0.02554550798784269</v>
+      </c>
+      <c r="T23">
+        <v>0.2376083114873622</v>
+      </c>
+      <c r="U23">
+        <v>0.1507388802649037</v>
+      </c>
+      <c r="V23">
+        <v>0.06359178652054678</v>
+      </c>
+      <c r="W23">
         <v>1</v>
       </c>
     </row>

</xml_diff>